<commit_message>
add cgi step for the search directory
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
     <sheet name="CAT" sheetId="1" r:id="rId2"/>
     <sheet name="CIM" sheetId="2" r:id="rId3"/>
-    <sheet name="Include-CGIs" sheetId="7" r:id="rId4"/>
+    <sheet name="-Include-CGIs" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="61">
   <si>
     <t>git</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>#include</t>
+  </si>
+  <si>
+    <t>/web/search/index.cgi</t>
+  </si>
+  <si>
+    <t>chmod 750 ./web/search/index.cgi</t>
   </si>
 </sst>
 </file>
@@ -1063,10 +1069,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A3:D26"/>
+  <dimension ref="A3:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,64 +1262,85 @@
       <c r="D16" s="28"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>35</v>
+      <c r="A17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="D17" s="28"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>29</v>
+      <c r="A18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>60</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="28"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="28"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B21" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="11"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
+      <c r="B23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-    </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1324,10 +1351,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,57 +1457,69 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="11"/>
+        <v>59</v>
+      </c>
+      <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>29</v>
+      <c r="A10" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>60</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1490,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D6"/>
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,23 +1606,37 @@
       <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
+      <c r="A7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="D9"/>
-    </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="D10"/>
+      <c r="A8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="28"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -1599,6 +1652,16 @@
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="D13"/>
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="4"/>
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="4"/>
+      <c r="D15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Set file permissions for /flashuploader/courseleaf.cgi
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
   <si>
     <t>git</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>/web/ribbit/index.cgi</t>
+  </si>
+  <si>
+    <t>chmod 750 ./web/&lt;progDir&gt;/flashuploader/courseleaf.cgi</t>
   </si>
 </sst>
 </file>
@@ -1075,54 +1078,66 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A3:D34"/>
+  <dimension ref="A2:D34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B2" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D2" s="21" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>10</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>37</v>
@@ -1407,7 +1422,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Commented out the cgi updates for the search directory
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="66">
   <si>
     <t>git</t>
   </si>
@@ -224,6 +224,12 @@
   </si>
   <si>
     <t>chmod 750 ./web/&lt;progDir&gt;/flashuploader/courseleaf.cgi</t>
+  </si>
+  <si>
+    <t>*cgi</t>
+  </si>
+  <si>
+    <t>*command</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1087,7 @@
   <dimension ref="A2:D34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A22" sqref="A22:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1338,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B22" s="47" t="s">
         <v>8</v>
@@ -1344,7 +1350,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B23" s="48" t="s">
         <v>60</v>
@@ -1423,7 +1429,7 @@
   <dimension ref="A2:D20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,7 +1580,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B14" s="47" t="s">
         <v>8</v>
@@ -1586,7 +1592,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Physically remove the search index.cgi records
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="CIM" sheetId="2" r:id="rId3"/>
     <sheet name="-Include-CGIs" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="64">
   <si>
     <t>git</t>
   </si>
@@ -224,12 +224,6 @@
   </si>
   <si>
     <t>chmod 750 ./web/&lt;progDir&gt;/flashuploader/courseleaf.cgi</t>
-  </si>
-  <si>
-    <t>*cgi</t>
-  </si>
-  <si>
-    <t>*command</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1078,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:D34"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A23"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,85 +1331,61 @@
       <c r="D21" s="28"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>59</v>
-      </c>
+      <c r="A22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="28"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>60</v>
+      <c r="A23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="28"/>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="28"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="11"/>
+      <c r="B27" s="8"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1426,10 +1396,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:D20"/>
+  <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,67 +1549,43 @@
       <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>59</v>
-      </c>
+      <c r="A14" s="16"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="28"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="48" t="s">
-        <v>60</v>
+      <c r="A15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="28"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="11"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added search directory cgi refresh
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="65">
   <si>
     <t>git</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>chmod 750 ./web/&lt;progDir&gt;/flashuploader/courseleaf.cgi</t>
+  </si>
+  <si>
+    <t>searchCgi</t>
   </si>
 </sst>
 </file>
@@ -1078,10 +1081,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:D32"/>
+  <dimension ref="A2:D34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,61 +1334,85 @@
       <c r="D21" s="28"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28"/>
+      <c r="A22" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>29</v>
+      <c r="A23" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>60</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="28"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B27" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1398,8 +1425,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added search to cim product defs
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="65">
   <si>
     <t>git</t>
   </si>
@@ -1083,8 +1083,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:D34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,10 +1423,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:D18"/>
+  <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,43 +1576,67 @@
       <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="28"/>
+      <c r="A14" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>29</v>
+      <c r="A15" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>60</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="28"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" s="11"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added a pdfgen 'product'
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
     <sheet name="cat" sheetId="1" r:id="rId2"/>
     <sheet name="cim" sheetId="2" r:id="rId3"/>
-    <sheet name="formbuilder" sheetId="8" r:id="rId4"/>
-    <sheet name="-Include-CGIs" sheetId="7" state="hidden" r:id="rId5"/>
+    <sheet name="pdfgen" sheetId="9" r:id="rId4"/>
+    <sheet name="formbuilder" sheetId="8" r:id="rId5"/>
+    <sheet name="-Include-CGIs" sheetId="7" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="65">
   <si>
     <t>git</t>
   </si>
@@ -1426,7 +1427,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -1646,6 +1647,81 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="D10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D4"/>
   <sheetViews>
@@ -1701,7 +1777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D15"/>
   <sheetViews>

</xml_diff>

<commit_message>
move where the /bin/fop is processed in pdfgen
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="74">
   <si>
     <t>git</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>/web/&lt;progDir&gt;/fop.xconf</t>
+  </si>
+  <si>
+    <t>#skeleton</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1117,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1647,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,25 +1692,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="25"/>
+        <v>67</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D5" s="25"/>
     </row>
@@ -1716,34 +1721,39 @@
         <v>32</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>68</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
-      <c r="D9"/>
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>

</xml_diff>

<commit_message>
removed the cfg file from pdggen
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="71">
   <si>
     <t>git</t>
   </si>
@@ -241,16 +241,13 @@
     <t xml:space="preserve">skeleton </t>
   </si>
   <si>
-    <t>warn</t>
-  </si>
-  <si>
-    <t>/web/admin/pdf.cfg</t>
-  </si>
-  <si>
     <t>include</t>
   </si>
   <si>
     <t>pdfgen</t>
+  </si>
+  <si>
+    <t>report</t>
   </si>
 </sst>
 </file>
@@ -1205,10 +1202,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="25"/>
@@ -1275,7 +1272,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>35</v>
@@ -1431,7 +1428,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>35</v>
@@ -1642,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,30 +1716,16 @@
         <v>67</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
       <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="D9"/>
+      <c r="D8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Make /bin/fop a compare/report for pdfgen
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="72">
   <si>
     <t>git</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>report</t>
+  </si>
+  <si>
+    <t>#skeleton</t>
   </si>
 </sst>
 </file>
@@ -1639,10 +1642,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1686,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>66</v>
@@ -1695,37 +1698,51 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D7" s="25" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
-      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="D9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update permissions on flashloader always
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="73">
   <si>
     <t>git</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>#skeleton</t>
+  </si>
+  <si>
+    <t>always</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1114,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1174,7 @@
         <v>61</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D5" s="18"/>
     </row>
@@ -1644,7 +1647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updtated to inclue the formbuilder sub product instead of hardcoding
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="74">
   <si>
     <t>git</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>always</t>
+  </si>
+  <si>
+    <t>formbuilder</t>
   </si>
 </sst>
 </file>
@@ -1114,8 +1117,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,17 +1197,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>10</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
@@ -1345,7 +1344,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1396,17 +1395,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>10</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
@@ -1639,7 +1634,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1647,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1735,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1758,7 +1756,7 @@
   <dimension ref="A2:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update searchGCgi record to use index.cgi
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -1490,7 +1490,7 @@
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1568,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Fix ribbit record in the cim section.
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="75">
   <si>
     <t>git</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>index.cgi</t>
+  </si>
+  <si>
+    <t>chmod 750 ./web/ribbit/index.cgi</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1357,7 @@
   <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1559,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>36</v>
@@ -1731,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
remove the command to set permissions on the /search/index.cgi file
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="75">
   <si>
     <t>git</t>
   </si>
@@ -1490,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D15"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,37 +1579,25 @@
       <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="28"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
+      <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1734,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update git directives to include the target directory
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="77">
   <si>
     <t>git</t>
   </si>
@@ -39,12 +39,6 @@
   </si>
   <si>
     <t>cgi</t>
-  </si>
-  <si>
-    <t>/web/courseleaf</t>
-  </si>
-  <si>
-    <t>/web</t>
   </si>
   <si>
     <t>/web/courseleaf/fonts</t>
@@ -260,6 +254,18 @@
   </si>
   <si>
     <t>chmod 750 ./web/ribbit/index.cgi</t>
+  </si>
+  <si>
+    <t>/web/&lt;progDir&gt;/ciim</t>
+  </si>
+  <si>
+    <t>/web/&lt;progDir&gt;/pdf</t>
+  </si>
+  <si>
+    <t>/web/&lt;progDir&gt;pdf</t>
+  </si>
+  <si>
+    <t>/web/&lt;progDir&gt;/formbuilder</t>
   </si>
 </sst>
 </file>
@@ -978,7 +984,7 @@
     </row>
     <row r="2" spans="2:4" s="6" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="36"/>
     </row>
@@ -991,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -1004,7 +1010,7 @@
     </row>
     <row r="7" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="30"/>
     </row>
@@ -1013,62 +1019,62 @@
         <v>1</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="32"/>
     </row>
     <row r="9" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="42" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" s="32"/>
     </row>
     <row r="10" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="43" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="32"/>
     </row>
     <row r="11" spans="2:4" s="31" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="43"/>
       <c r="C11" s="37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="32"/>
     </row>
     <row r="12" spans="2:4" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="43"/>
       <c r="C12" s="37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" s="32"/>
     </row>
     <row r="13" spans="2:4" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="43"/>
       <c r="C13" s="37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="32"/>
     </row>
     <row r="14" spans="2:4" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="43"/>
       <c r="C14" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="32"/>
     </row>
     <row r="15" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="32"/>
     </row>
@@ -1078,7 +1084,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="40"/>
     </row>
@@ -1088,18 +1094,18 @@
     </row>
     <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="40" t="s">
         <v>40</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="40" t="s">
         <v>41</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -1121,7 +1127,7 @@
   <dimension ref="A2:D26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,13 +1143,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1151,36 +1157,36 @@
         <v>0</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" s="18"/>
     </row>
@@ -1189,31 +1195,31 @@
         <v>0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="25"/>
@@ -1226,49 +1232,49 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D13" s="11"/>
     </row>
@@ -1280,10 +1286,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
@@ -1296,13 +1302,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17" s="11"/>
     </row>
@@ -1314,13 +1320,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" s="11"/>
     </row>
@@ -1357,7 +1363,7 @@
   <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,13 +1379,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1387,21 +1393,21 @@
         <v>0</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="25"/>
@@ -1414,13 +1420,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" s="25"/>
     </row>
@@ -1432,10 +1438,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
@@ -1448,13 +1454,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="11"/>
     </row>
@@ -1466,13 +1472,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="11"/>
     </row>
@@ -1492,7 +1498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -1509,13 +1515,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1523,22 +1529,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -1547,34 +1553,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="11"/>
     </row>
@@ -1610,7 +1616,7 @@
   <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,13 +1632,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1640,65 +1646,65 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="D7" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1722,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,13 +1745,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1753,13 +1759,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,13 +1801,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1809,22 +1815,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -1833,22 +1839,22 @@
         <v>2</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="28"/>
     </row>
@@ -1857,22 +1863,22 @@
         <v>2</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="28"/>
     </row>

</xml_diff>

<commit_message>
fix problem with cim git definition
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -256,16 +256,16 @@
     <t>chmod 750 ./web/ribbit/index.cgi</t>
   </si>
   <si>
-    <t>/web/&lt;progDir&gt;/ciim</t>
-  </si>
-  <si>
-    <t>/web/&lt;progDir&gt;pdf</t>
+    <t>/web/&lt;progDir&gt;/pdf</t>
   </si>
   <si>
     <t>/web/&lt;progDir&gt;/formbuilder</t>
   </si>
   <si>
     <t>/web/&lt;progDir&gt;/navmaster</t>
+  </si>
+  <si>
+    <t>/web/&lt;progDir&gt;/cim</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1198,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>8</v>
@@ -1360,10 +1360,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,7 +1396,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>8</v>
@@ -1413,80 +1413,62 @@
       <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="A5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="25"/>
+        <v>33</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
+      <c r="A7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="A8" s="16"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="28"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="28"/>
+      <c r="A9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="28"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1649,7 +1631,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>8</v>
@@ -1762,7 +1744,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fix problem with email specifications in cat
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="78">
   <si>
     <t>git</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>/web/&lt;progDir&gt;</t>
-  </si>
-  <si>
-    <t>/web/&lt;progDir&gt;/js</t>
   </si>
   <si>
     <t>/bin/daily.sh</t>
@@ -199,9 +196,6 @@
     <t>/email</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>/web/search/index.cgi</t>
   </si>
   <si>
@@ -266,6 +260,15 @@
   </si>
   <si>
     <t>/web/&lt;progDir&gt;/cim</t>
+  </si>
+  <si>
+    <t>/web/&lt;progDir&gt;/fonts</t>
+  </si>
+  <si>
+    <t>/web/&lt;progDir&gt;/js/ckeditor</t>
+  </si>
+  <si>
+    <t>/web/&lt;progDir&gt;/focussearch</t>
   </si>
 </sst>
 </file>
@@ -968,7 +971,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:D21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -997,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -1010,7 +1013,7 @@
     </row>
     <row r="7" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="30"/>
     </row>
@@ -1044,28 +1047,28 @@
     <row r="11" spans="2:4" s="31" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="43"/>
       <c r="C11" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="32"/>
     </row>
     <row r="12" spans="2:4" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="43"/>
       <c r="C12" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="32"/>
     </row>
     <row r="13" spans="2:4" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="43"/>
       <c r="C13" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="32"/>
     </row>
     <row r="14" spans="2:4" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="43"/>
       <c r="C14" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="32"/>
     </row>
@@ -1084,7 +1087,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="40"/>
     </row>
@@ -1094,18 +1097,18 @@
     </row>
     <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -1126,8 +1129,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1168,25 +1171,25 @@
     </row>
     <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>48</v>
-      </c>
       <c r="C4" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" s="18"/>
     </row>
@@ -1198,7 +1201,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>8</v>
@@ -1206,20 +1209,20 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="25"/>
@@ -1232,49 +1235,49 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="C12" s="10" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D13" s="11"/>
     </row>
@@ -1286,10 +1289,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
@@ -1305,10 +1308,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="11"/>
     </row>
@@ -1320,10 +1323,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>10</v>
@@ -1379,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1396,7 +1399,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>8</v>
@@ -1404,32 +1407,32 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
@@ -1439,10 +1442,10 @@
         <v>16</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="11"/>
     </row>
@@ -1454,10 +1457,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>10</v>
@@ -1497,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1511,22 +1514,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -1535,34 +1538,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="11"/>
     </row>
@@ -1614,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1631,7 +1634,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>8</v>
@@ -1639,54 +1642,54 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="D7" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1727,7 +1730,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1741,10 +1744,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>8</v>
@@ -1783,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1797,22 +1800,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -1830,13 +1833,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="28"/>
     </row>
@@ -1848,19 +1851,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="28"/>
     </row>

</xml_diff>

<commit_message>
Added /courseleaf/fonts to cim
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControl.xlsx
+++ b/workbooks/courseleafPatchControl.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
   <si>
     <t>git</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>skeleton</t>
-  </si>
-  <si>
-    <t>/web/courseleaf/focussearch</t>
   </si>
   <si>
     <t>Pattern (see instructions sheet)</t>
@@ -266,9 +263,6 @@
   </si>
   <si>
     <t>/web/&lt;progDir&gt;/js/ckeditor</t>
-  </si>
-  <si>
-    <t>/web/&lt;progDir&gt;/focussearch</t>
   </si>
 </sst>
 </file>
@@ -972,7 +966,7 @@
   <dimension ref="B1:D21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -1013,7 +1007,7 @@
     </row>
     <row r="7" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="30"/>
     </row>
@@ -1047,28 +1041,28 @@
     <row r="11" spans="2:4" s="31" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="43"/>
       <c r="C11" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="32"/>
     </row>
     <row r="12" spans="2:4" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="43"/>
       <c r="C12" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="32"/>
     </row>
     <row r="13" spans="2:4" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="43"/>
       <c r="C13" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="32"/>
     </row>
     <row r="14" spans="2:4" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="43"/>
       <c r="C14" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="32"/>
     </row>
@@ -1087,7 +1081,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="40"/>
     </row>
@@ -1097,18 +1091,18 @@
     </row>
     <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -1127,10 +1121,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:D26"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1171,25 +1165,25 @@
     </row>
     <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>47</v>
-      </c>
       <c r="C4" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="18"/>
     </row>
@@ -1201,7 +1195,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>8</v>
@@ -1209,20 +1203,20 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>64</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="25"/>
@@ -1241,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" s="11"/>
     </row>
@@ -1253,7 +1247,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="11"/>
     </row>
@@ -1262,97 +1256,85 @@
         <v>29</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>52</v>
-      </c>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>32</v>
-      </c>
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
+      <c r="A16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="11"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
+      <c r="B20" s="8"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1363,10 +1345,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:D10"/>
+  <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1399,7 +1381,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>8</v>
@@ -1407,10 +1389,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="25"/>
@@ -1420,58 +1402,70 @@
         <v>29</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="28"/>
+      <c r="C8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1500,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1514,7 +1508,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>27</v>
@@ -1523,13 +1517,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -1538,34 +1532,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="11"/>
     </row>
@@ -1617,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1634,7 +1628,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>8</v>
@@ -1642,28 +1636,28 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,25 +1665,25 @@
         <v>29</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1730,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1744,10 +1738,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>8</v>
@@ -1786,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>7</v>
@@ -1800,7 +1794,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>27</v>
@@ -1809,13 +1803,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -1833,13 +1827,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="28"/>
     </row>
@@ -1851,19 +1845,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="28"/>
     </row>

</xml_diff>